<commit_message>
added page fans in plot
</commit_message>
<xml_diff>
--- a/excels/lite/RegionDF_countinuously.xlsx
+++ b/excels/lite/RegionDF_countinuously.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Date Fetched</t>
   </si>
@@ -23,9 +28,6 @@
   </si>
   <si>
     <t>Fans</t>
-  </si>
-  <si>
-    <t>19/03/2019</t>
   </si>
   <si>
     <t>Central Macedonia, Greece</t>
@@ -52,20 +54,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -81,15 +82,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -377,18 +380,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -402,160 +401,165 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" s="1">
+        <v>43542</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>43542</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>43542</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>43542</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>43542</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>43542</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>43542</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>43543</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>43543</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>43543</v>
+      </c>
+      <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>43543</v>
+      </c>
+      <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>43543</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>43543</v>
+      </c>
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>43543</v>
+      </c>
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="C15">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="n">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="n">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hacked excels with 23/4 added
</commit_message>
<xml_diff>
--- a/excels/lite/RegionDF_countinuously.xlsx
+++ b/excels/lite/RegionDF_countinuously.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="12">
   <si>
     <t>Date Fetched</t>
   </si>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C330"/>
+  <dimension ref="A1:C337"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
-      <selection activeCell="A330" sqref="A330"/>
+      <selection activeCell="C332" sqref="C332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4058,6 +4058,83 @@
         <v>15</v>
       </c>
     </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A331" s="1">
+        <v>43578</v>
+      </c>
+      <c r="B331" t="s">
+        <v>4</v>
+      </c>
+      <c r="C331">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A332" s="1">
+        <v>43578</v>
+      </c>
+      <c r="B332" t="s">
+        <v>3</v>
+      </c>
+      <c r="C332">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A333" s="1">
+        <v>43578</v>
+      </c>
+      <c r="B333" t="s">
+        <v>6</v>
+      </c>
+      <c r="C333">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A334" s="1">
+        <v>43578</v>
+      </c>
+      <c r="B334" t="s">
+        <v>5</v>
+      </c>
+      <c r="C334">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A335" s="1">
+        <v>43578</v>
+      </c>
+      <c r="B335" t="s">
+        <v>10</v>
+      </c>
+      <c r="C335">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A336" s="1">
+        <v>43578</v>
+      </c>
+      <c r="B336" t="s">
+        <v>8</v>
+      </c>
+      <c r="C336">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A337" s="1">
+        <v>43578</v>
+      </c>
+      <c r="B337" t="s">
+        <v>7</v>
+      </c>
+      <c r="C337">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>